<commit_message>
merged final LLm dev version to the master branch
</commit_message>
<xml_diff>
--- a/data/Resources Version 3.xlsx
+++ b/data/Resources Version 3.xlsx
@@ -547,7 +547,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>8713562192546900832</t>
+          <t>-4669408271107115015</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>-1541966203449101404</t>
+          <t>2562344382223594109</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>3636439332915921703</t>
+          <t>1335659840519498668</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>-1571738145923170822</t>
+          <t>5996603765422949120</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>3813825339775659397</t>
+          <t>-6998875974584128087</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>7590268731239541923</t>
+          <t>-5475145229998163696</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>-2732430653382116429</t>
+          <t>-2835556762357383323</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2219353666286793304</t>
+          <t>3446381195598226073</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>4715990202116755095</t>
+          <t>7429004412795776543</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-8053399616633296484</t>
+          <t>-7463789233438201725</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>-2960455000518483943</t>
+          <t>4027219914018584327</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>5139825118934878628</t>
+          <t>-4674392798130057955</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>3438138152516692476</t>
+          <t>-7637377842190785896</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>-7771810733523564428</t>
+          <t>-7281215925882653879</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>-6383168384813898071</t>
+          <t>-9187606730424740507</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>-7546633456481591208</t>
+          <t>-9052204443863224496</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>-4464855400474175518</t>
+          <t>3565369082796405098</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>-7486836821201046316</t>
+          <t>5383642578937811772</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1335300087221315275</t>
+          <t>1813757887779950780</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>4890396292687318694</t>
+          <t>-3053584235034484636</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>-6773162375628834220</t>
+          <t>5774924842076293986</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>-1357622733001855587</t>
+          <t>-7542380756249618802</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>-8273623228730885961</t>
+          <t>3802420700669269005</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2937325645292590715</t>
+          <t>-7510689911077507317</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>5793214142440861976</t>
+          <t>4092745595163590294</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>-6626977058051633297</t>
+          <t>5931376669348687862</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>1790404095933201453</t>
+          <t>-5940024129707403889</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>5217164969088571035</t>
+          <t>4364507000682221330</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>3724060929283708654</t>
+          <t>-6251822611627381820</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>6734150183421995532</t>
+          <t>9194370770878731756</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>-6040830167132545308</t>
+          <t>-2573120143148544423</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>-659307792757818048</t>
+          <t>-2922135161630420216</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>7754225662788753075</t>
+          <t>-4061181764622731611</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>-2132883670212164973</t>
+          <t>9148675668092575960</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>-1832039145102797619</t>
+          <t>6527780559740483419</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>5457253959279844934</t>
+          <t>3251194705625389330</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>-9062013516978961721</t>
+          <t>-5865924292979335865</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>4373771730686011710</t>
+          <t>983837149220240218</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>5753125056368312992</t>
+          <t>-8178142439609417894</t>
         </is>
       </c>
     </row>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>6543031714245386642</t>
+          <t>-1982624170970766400</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>8785419633867862118</t>
+          <t>4273187226288731122</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>-4930189140315237194</t>
+          <t>-7823256271156071639</t>
         </is>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>-7356763855637023544</t>
+          <t>-5389380374220094127</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>8339983490650982846</t>
+          <t>842808910147666040</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>-2849223929302928029</t>
+          <t>-7027520035701953342</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>-3238483086538196895</t>
+          <t>7482896755199130411</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>4994160590979564638</t>
+          <t>398461538887469177</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>-6737764714683581729</t>
+          <t>3454457610105064551</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>1369169707740040964</t>
+          <t>7975526024234341400</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>3089404974594477887</t>
+          <t>-9074573913476167943</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>632168737504649034</t>
+          <t>-7644393027888801605</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>-4808705032324583248</t>
+          <t>-8736609244716448440</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>-2261164552961112249</t>
+          <t>9052369947022218863</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>3841358117306543570</t>
+          <t>3353293156645676120</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>-2826230110091421206</t>
+          <t>4141321283835704752</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>7966925184486280147</t>
+          <t>8665801438741787055</t>
         </is>
       </c>
     </row>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>4460213425018821355</t>
+          <t>8026515781360407232</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>-5875932483433407387</t>
+          <t>-1932180419715559172</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>1528296703883395032</t>
+          <t>-6401688029597286219</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>-8132867534885983830</t>
+          <t>-3675364794334992712</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>4457055390951487489</t>
+          <t>-9041070344155293603</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>-2386463039136446109</t>
+          <t>827234789837150651</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>-3704268701197480870</t>
+          <t>2896951924815176809</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>7071519757944210242</t>
+          <t>-4564927636733383673</t>
         </is>
       </c>
     </row>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>-7151945327819675204</t>
+          <t>4346095948121300196</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>866159219613002274</t>
+          <t>1065943385603141873</t>
         </is>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>8388034325410465279</t>
+          <t>-5278807518909587042</t>
         </is>
       </c>
     </row>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>3164634883554010995</t>
+          <t>-5835854445242952712</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>-5423001504316218678</t>
+          <t>-6822358234754472967</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>5542935612129473013</t>
+          <t>3708082281646037747</t>
         </is>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>-3043391571894132726</t>
+          <t>-8265658807534808874</t>
         </is>
       </c>
     </row>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>2567146970219707473</t>
+          <t>7099134179675151626</t>
         </is>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>575821806591374094</t>
+          <t>3356488155610174055</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>9036053113795199263</t>
+          <t>-4462617100031512972</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>-2658184405269711623</t>
+          <t>6448256386941056123</t>
         </is>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>-4498586851639602311</t>
+          <t>-7554034832876654556</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>-6424443751316579744</t>
+          <t>-7651780901050156358</t>
         </is>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>7422438715592695282</t>
+          <t>-5242002038649732807</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>-2264251119609981777</t>
+          <t>-7223094674867632695</t>
         </is>
       </c>
     </row>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>3969834520324838311</t>
+          <t>-4758225081747388329</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>-7009602871683778770</t>
+          <t>-6471016732082741431</t>
         </is>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>-449665683281509008</t>
+          <t>-1532218457583809050</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>8830372953235301604</t>
+          <t>-7830903407751587634</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>-5736646082072081081</t>
+          <t>607982924321726346</t>
         </is>
       </c>
     </row>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>8496066456718679662</t>
+          <t>2931331187289253624</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>396823090042982428</t>
+          <t>-6608270988803108268</t>
         </is>
       </c>
     </row>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>-5440532276700012036</t>
+          <t>-3545368066328936975</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>7471178938802190776</t>
+          <t>-8245609285263173720</t>
         </is>
       </c>
     </row>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>-1974473612037538092</t>
+          <t>-6817527042806302098</t>
         </is>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>-5741035770819957472</t>
+          <t>4226159402944338817</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>2551687562996255016</t>
+          <t>-8733751989412479732</t>
         </is>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>-8537664900403988036</t>
+          <t>2135284477141067564</t>
         </is>
       </c>
     </row>
@@ -5799,7 +5799,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>828780839150458077</t>
+          <t>8547637798006313293</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>-2462430459142764899</t>
+          <t>-1725801069015490380</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>-2449014321636352010</t>
+          <t>-6259110673509628006</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>-5466430580012110641</t>
+          <t>-6632695896113477861</t>
         </is>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>2963684312909574439</t>
+          <t>371515243498320495</t>
         </is>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>5085501326381886668</t>
+          <t>-6645619232178745875</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>2907857480426639049</t>
+          <t>6915134116159647783</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>7650004842871796274</t>
+          <t>2032903072489254546</t>
         </is>
       </c>
     </row>
@@ -6247,7 +6247,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>4179706748142790720</t>
+          <t>6659997813533707755</t>
         </is>
       </c>
     </row>
@@ -6303,7 +6303,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>-7915630495634216174</t>
+          <t>6944677855127498614</t>
         </is>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>-2463235316568851138</t>
+          <t>-7061210741146999748</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>9065837698206883647</t>
+          <t>-4538597036795211515</t>
         </is>
       </c>
     </row>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>4609050877155203916</t>
+          <t>2085552372673337609</t>
         </is>
       </c>
     </row>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>-7419841051507337819</t>
+          <t>-3280993061587374113</t>
         </is>
       </c>
     </row>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>4753742916144407003</t>
+          <t>2898198441661816279</t>
         </is>
       </c>
     </row>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>-2818908291271500995</t>
+          <t>-2909176430954739216</t>
         </is>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>-9232773276089606</t>
+          <t>-2711444929100397157</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>-642242584758324067</t>
+          <t>4956504020497059340</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>6495160006822576224</t>
+          <t>-7983552625542901343</t>
         </is>
       </c>
     </row>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>-8380829630876370401</t>
+          <t>4091129384689248972</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>-4669197101343577074</t>
+          <t>-2077921111104666513</t>
         </is>
       </c>
     </row>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>8817355325900065615</t>
+          <t>1481385744804257218</t>
         </is>
       </c>
     </row>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>4974899086889878718</t>
+          <t>-1314268846930609699</t>
         </is>
       </c>
     </row>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>1297440786639002181</t>
+          <t>-4762969570010234327</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>6185465424342073383</t>
+          <t>4686133869367337438</t>
         </is>
       </c>
     </row>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>-1031938082639394071</t>
+          <t>-1314376077306140276</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>-6598817914450491803</t>
+          <t>1952707532589046991</t>
         </is>
       </c>
     </row>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>2945376191230423512</t>
+          <t>-1655257064869950209</t>
         </is>
       </c>
     </row>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>-4302803611391401951</t>
+          <t>7211243743205361964</t>
         </is>
       </c>
     </row>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>-3703718792834571921</t>
+          <t>-1397029152657909876</t>
         </is>
       </c>
     </row>
@@ -7499,7 +7499,7 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>-3391450705165916627</t>
+          <t>-2957664614295267829</t>
         </is>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>8445961029932370432</t>
+          <t>-1019300093287602957</t>
         </is>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>-9142168250756759206</t>
+          <t>5083804542754861460</t>
         </is>
       </c>
     </row>
@@ -7673,7 +7673,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>7736456355242828385</t>
+          <t>-684667185360629911</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>7347078206698453342</t>
+          <t>2181380623218178445</t>
         </is>
       </c>
     </row>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>-4862230572593322762</t>
+          <t>8595903504432045558</t>
         </is>
       </c>
     </row>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>3946782044117994561</t>
+          <t>-1819096483199804492</t>
         </is>
       </c>
     </row>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>2967813001932044278</t>
+          <t>-2522337984013915347</t>
         </is>
       </c>
     </row>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>-7274218586611233388</t>
+          <t>-3447057015283101846</t>
         </is>
       </c>
     </row>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>5782455830463891967</t>
+          <t>1715740541100954805</t>
         </is>
       </c>
     </row>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>168595899885866963</t>
+          <t>-8336191736962316114</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>-189983657313535992</t>
+          <t>1530903909874727812</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>964393088601274918</t>
+          <t>-6617530120066595529</t>
         </is>
       </c>
     </row>
@@ -8247,7 +8247,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>4834275600412885784</t>
+          <t>-3630915378332725157</t>
         </is>
       </c>
     </row>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>4516830995210478123</t>
+          <t>6766916804570629763</t>
         </is>
       </c>
     </row>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>7177332859778505296</t>
+          <t>-6102625487373628845</t>
         </is>
       </c>
     </row>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>4227276425330492922</t>
+          <t>-6427175365258669468</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>2085566140709304802</t>
+          <t>8868946038062910910</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>2722080269005689777</t>
+          <t>7595204490086872621</t>
         </is>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>-2288810810110725278</t>
+          <t>-2207655033940450072</t>
         </is>
       </c>
     </row>
@@ -8653,7 +8653,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>2982174338762573132</t>
+          <t>-4322783782782921251</t>
         </is>
       </c>
     </row>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>-4358139017262951319</t>
+          <t>-231162873458323514</t>
         </is>
       </c>
     </row>
@@ -8769,7 +8769,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>2603475284036405681</t>
+          <t>7050037241090277956</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>849095821221820012</t>
+          <t>-7873238011731733162</t>
         </is>
       </c>
     </row>
@@ -8881,7 +8881,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>-4543347885647006786</t>
+          <t>-5941049182536849109</t>
         </is>
       </c>
     </row>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>-6543130930797442440</t>
+          <t>-8620407933545991259</t>
         </is>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>-8824300036632286886</t>
+          <t>-559472240420349259</t>
         </is>
       </c>
     </row>
@@ -9055,7 +9055,7 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>5818292807362776608</t>
+          <t>-4981140518067300793</t>
         </is>
       </c>
     </row>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>6513497332292919279</t>
+          <t>643542772026338771</t>
         </is>
       </c>
     </row>
@@ -9167,7 +9167,7 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>709282409001652438</t>
+          <t>3268863545090775617</t>
         </is>
       </c>
     </row>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>4701839046558553810</t>
+          <t>2672343686471530480</t>
         </is>
       </c>
     </row>
@@ -9279,7 +9279,7 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>-8899730283588130001</t>
+          <t>-3643599378168043464</t>
         </is>
       </c>
     </row>
@@ -9335,7 +9335,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>3873515907134056814</t>
+          <t>6434209926653554900</t>
         </is>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>4250101266499834803</t>
+          <t>-1270118825763535676</t>
         </is>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>4411890456388680342</t>
+          <t>5429892603301549684</t>
         </is>
       </c>
     </row>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>6145948822230621177</t>
+          <t>-8894611048198543196</t>
         </is>
       </c>
     </row>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>-8942787840726369782</t>
+          <t>-2160264276138159527</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>930480290792908829</t>
+          <t>-8474327674694741285</t>
         </is>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>899904477480659529</t>
+          <t>246140732267578233</t>
         </is>
       </c>
     </row>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>-8863058488880161092</t>
+          <t>-1129151466573563612</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>5490689411403517575</t>
+          <t>9205179774127900571</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>-2844904823292744522</t>
+          <t>-2364160728764779491</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>-7298690349340408211</t>
+          <t>8108395386256394258</t>
         </is>
       </c>
     </row>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>7995458440462091846</t>
+          <t>-954166402165324989</t>
         </is>
       </c>
     </row>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>6578518925165244088</t>
+          <t>543821272980740781</t>
         </is>
       </c>
     </row>
@@ -10081,7 +10081,7 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>6107474619945933555</t>
+          <t>8546088309797410840</t>
         </is>
       </c>
     </row>
@@ -10139,7 +10139,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>-3362657266703223321</t>
+          <t>444406988666437715</t>
         </is>
       </c>
     </row>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>4441029628017113004</t>
+          <t>6674371758819296065</t>
         </is>
       </c>
     </row>
@@ -10253,7 +10253,7 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>-7198329183230474046</t>
+          <t>-5504371936227284663</t>
         </is>
       </c>
     </row>
@@ -10309,7 +10309,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>511219117999284682</t>
+          <t>6352385770273794128</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>-4794723507219520131</t>
+          <t>-9032907689358954166</t>
         </is>
       </c>
     </row>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>4500580161779930098</t>
+          <t>-6541113570474471252</t>
         </is>
       </c>
     </row>
@@ -10479,7 +10479,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>-1101049693910055706</t>
+          <t>1401012005982569654</t>
         </is>
       </c>
     </row>
@@ -10537,7 +10537,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>2395480335321541350</t>
+          <t>-1292458585129911830</t>
         </is>
       </c>
     </row>
@@ -10595,7 +10595,7 @@
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>-227338227260717135</t>
+          <t>8697378646641891277</t>
         </is>
       </c>
     </row>
@@ -10653,7 +10653,7 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>-3079354575994856488</t>
+          <t>6179180593092849479</t>
         </is>
       </c>
     </row>
@@ -10711,7 +10711,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>7981956716870496133</t>
+          <t>6365682726562351476</t>
         </is>
       </c>
     </row>
@@ -10769,7 +10769,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>-4459992789199129341</t>
+          <t>8164388562393133545</t>
         </is>
       </c>
     </row>
@@ -10827,7 +10827,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>-1700574594681705468</t>
+          <t>-721850228734678966</t>
         </is>
       </c>
     </row>
@@ -10885,7 +10885,7 @@
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>-6848709344473618967</t>
+          <t>-8049177185306195896</t>
         </is>
       </c>
     </row>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>56482740254729</t>
+          <t>-6309357319046325101</t>
         </is>
       </c>
     </row>
@@ -10997,7 +10997,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>-5498758887376538349</t>
+          <t>-518677825884927479</t>
         </is>
       </c>
     </row>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>-1693876697400247719</t>
+          <t>-6928029703104404322</t>
         </is>
       </c>
     </row>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>-4610229845133376692</t>
+          <t>4579203732849881173</t>
         </is>
       </c>
     </row>
@@ -11171,7 +11171,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>4203573616813512320</t>
+          <t>5728739737985536577</t>
         </is>
       </c>
     </row>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>167253594939819874</t>
+          <t>8216443390237770815</t>
         </is>
       </c>
     </row>
@@ -11283,7 +11283,7 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>-5476507460861573723</t>
+          <t>1278822940952494633</t>
         </is>
       </c>
     </row>
@@ -11339,7 +11339,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>-8947038303407608728</t>
+          <t>4005647799575941891</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Source titles are added
</commit_message>
<xml_diff>
--- a/data/Resources Version 3.xlsx
+++ b/data/Resources Version 3.xlsx
@@ -547,7 +547,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>-4669408271107115015</t>
+          <t>3662640957984824165</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2562344382223594109</t>
+          <t>-2205727469830209581</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>1335659840519498668</t>
+          <t>3947032688143015583</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>5996603765422949120</t>
+          <t>-4070058339261262404</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>-6998875974584128087</t>
+          <t>3974254717169165242</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-5475145229998163696</t>
+          <t>-4561709708017358982</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>-2835556762357383323</t>
+          <t>1551291109968057236</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>3446381195598226073</t>
+          <t>-4518089163609736458</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>7429004412795776543</t>
+          <t>-3183684730125675937</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-7463789233438201725</t>
+          <t>-9168276457019987318</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>4027219914018584327</t>
+          <t>-4617949069363649069</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>-4674392798130057955</t>
+          <t>3493635241480552645</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>-7637377842190785896</t>
+          <t>4120352725638207378</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>-7281215925882653879</t>
+          <t>1520873511535781825</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>-9187606730424740507</t>
+          <t>6574711592521513742</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>-9052204443863224496</t>
+          <t>-8338804174920443849</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>3565369082796405098</t>
+          <t>312702367421235649</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>5383642578937811772</t>
+          <t>-5970054463927394358</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>1813757887779950780</t>
+          <t>-4263260082488223738</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>-3053584235034484636</t>
+          <t>-5612201309808146888</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>5774924842076293986</t>
+          <t>5145432123831290462</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>-7542380756249618802</t>
+          <t>1015697036543477830</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>3802420700669269005</t>
+          <t>-208326485726242567</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>-7510689911077507317</t>
+          <t>7646751089657057711</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>4092745595163590294</t>
+          <t>-5415919449685052607</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>5931376669348687862</t>
+          <t>7868390111142095063</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>-5940024129707403889</t>
+          <t>-7488405086253764194</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>4364507000682221330</t>
+          <t>-1861682879708476291</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>-6251822611627381820</t>
+          <t>-8847728220741545953</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>9194370770878731756</t>
+          <t>4457302807822112719</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>-2573120143148544423</t>
+          <t>-625322754259993442</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>-2922135161630420216</t>
+          <t>-3213279485514674737</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>-4061181764622731611</t>
+          <t>8404831805550815693</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>9148675668092575960</t>
+          <t>-8933857045255588965</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>6527780559740483419</t>
+          <t>5254168911598103324</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>3251194705625389330</t>
+          <t>-772281424943873119</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>-5865924292979335865</t>
+          <t>5497686737915771151</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>983837149220240218</t>
+          <t>-8007489703386405862</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>-8178142439609417894</t>
+          <t>-1224088264320340539</t>
         </is>
       </c>
     </row>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>-1982624170970766400</t>
+          <t>65550805372217523</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>4273187226288731122</t>
+          <t>3959022303982822678</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>-7823256271156071639</t>
+          <t>2893424119587123128</t>
         </is>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>-5389380374220094127</t>
+          <t>6729436500093376029</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>842808910147666040</t>
+          <t>-9092111020908679666</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>-7027520035701953342</t>
+          <t>-5776440433675510743</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>7482896755199130411</t>
+          <t>3289512220574743916</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>398461538887469177</t>
+          <t>-3912504612805688163</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>3454457610105064551</t>
+          <t>211745950761418373</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>7975526024234341400</t>
+          <t>-813659942172640462</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>-9074573913476167943</t>
+          <t>-280881007667315352</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>-7644393027888801605</t>
+          <t>-637642966314824375</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>-8736609244716448440</t>
+          <t>4018800685974547100</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>9052369947022218863</t>
+          <t>6425201151129509066</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>3353293156645676120</t>
+          <t>664692401615066690</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>4141321283835704752</t>
+          <t>1575136103729739998</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>8665801438741787055</t>
+          <t>-2557687514756119600</t>
         </is>
       </c>
     </row>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>8026515781360407232</t>
+          <t>-4299873427710969298</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>-1932180419715559172</t>
+          <t>-940197697172272793</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>-6401688029597286219</t>
+          <t>-6794072827604301818</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>-3675364794334992712</t>
+          <t>-8673794620469508205</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>-9041070344155293603</t>
+          <t>-781131645495908453</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>827234789837150651</t>
+          <t>-1330214522552559642</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>2896951924815176809</t>
+          <t>5774951135724176630</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>-4564927636733383673</t>
+          <t>-2492042789545590560</t>
         </is>
       </c>
     </row>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>4346095948121300196</t>
+          <t>5165846990965736332</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>1065943385603141873</t>
+          <t>3130469186114237930</t>
         </is>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>-5278807518909587042</t>
+          <t>-774411147450069977</t>
         </is>
       </c>
     </row>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>-5835854445242952712</t>
+          <t>-2650407188651912047</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>-6822358234754472967</t>
+          <t>-908987616845626214</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>3708082281646037747</t>
+          <t>-4060061898629540777</t>
         </is>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>-8265658807534808874</t>
+          <t>-4532436151914642469</t>
         </is>
       </c>
     </row>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>7099134179675151626</t>
+          <t>1459852186908969580</t>
         </is>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>3356488155610174055</t>
+          <t>6282601747389355345</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>-4462617100031512972</t>
+          <t>3519689203908794831</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>6448256386941056123</t>
+          <t>1638720622492765062</t>
         </is>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>-7554034832876654556</t>
+          <t>-8033667434504302137</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>-7651780901050156358</t>
+          <t>6751182094598153038</t>
         </is>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>-5242002038649732807</t>
+          <t>-5254112671037145471</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>-7223094674867632695</t>
+          <t>1076389866509198222</t>
         </is>
       </c>
     </row>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>-4758225081747388329</t>
+          <t>-2962127134674495331</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>-6471016732082741431</t>
+          <t>-4919118608278039778</t>
         </is>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>-1532218457583809050</t>
+          <t>-7231451410249793031</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>-7830903407751587634</t>
+          <t>1605600418937571350</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>607982924321726346</t>
+          <t>917846148114197462</t>
         </is>
       </c>
     </row>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>2931331187289253624</t>
+          <t>-6364450786823172080</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>-6608270988803108268</t>
+          <t>2924035588330404652</t>
         </is>
       </c>
     </row>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>-3545368066328936975</t>
+          <t>-5769097701753140988</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>-8245609285263173720</t>
+          <t>-8827049855292318136</t>
         </is>
       </c>
     </row>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>-6817527042806302098</t>
+          <t>4173045203913581098</t>
         </is>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>4226159402944338817</t>
+          <t>-5278319329484131655</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>-8733751989412479732</t>
+          <t>-1735731827933621612</t>
         </is>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>2135284477141067564</t>
+          <t>1952093456905376577</t>
         </is>
       </c>
     </row>
@@ -5799,7 +5799,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>8547637798006313293</t>
+          <t>2173678999482831795</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>-1725801069015490380</t>
+          <t>5900994253310099602</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>-6259110673509628006</t>
+          <t>5468280461743058903</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>-6632695896113477861</t>
+          <t>5992219105724045985</t>
         </is>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>371515243498320495</t>
+          <t>-855068379621288064</t>
         </is>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>-6645619232178745875</t>
+          <t>-7514884896793776053</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>6915134116159647783</t>
+          <t>-4007255360055736767</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>2032903072489254546</t>
+          <t>9051414917383599879</t>
         </is>
       </c>
     </row>
@@ -6247,7 +6247,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>6659997813533707755</t>
+          <t>-1180506624026339843</t>
         </is>
       </c>
     </row>
@@ -6303,7 +6303,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>6944677855127498614</t>
+          <t>-857840874557669554</t>
         </is>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>-7061210741146999748</t>
+          <t>-3207098703688345024</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>-4538597036795211515</t>
+          <t>-6880334182832083659</t>
         </is>
       </c>
     </row>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>2085552372673337609</t>
+          <t>-43504159787510576</t>
         </is>
       </c>
     </row>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>-3280993061587374113</t>
+          <t>101705950246348686</t>
         </is>
       </c>
     </row>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>2898198441661816279</t>
+          <t>-7616530941552643312</t>
         </is>
       </c>
     </row>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>-2909176430954739216</t>
+          <t>-7243990865538090742</t>
         </is>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>-2711444929100397157</t>
+          <t>-6331353430656479257</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>4956504020497059340</t>
+          <t>8261618368864195616</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>-7983552625542901343</t>
+          <t>-4462920339258683482</t>
         </is>
       </c>
     </row>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>4091129384689248972</t>
+          <t>1002060103863177932</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>-2077921111104666513</t>
+          <t>-8158071597057416025</t>
         </is>
       </c>
     </row>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>1481385744804257218</t>
+          <t>-8157904845361839123</t>
         </is>
       </c>
     </row>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>-1314268846930609699</t>
+          <t>-6026434707399987736</t>
         </is>
       </c>
     </row>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>-4762969570010234327</t>
+          <t>5596896287552915416</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>4686133869367337438</t>
+          <t>7014636261738343865</t>
         </is>
       </c>
     </row>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>-1314376077306140276</t>
+          <t>-1621598255050098166</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>1952707532589046991</t>
+          <t>1765071489886768529</t>
         </is>
       </c>
     </row>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>-1655257064869950209</t>
+          <t>-1644948235369330338</t>
         </is>
       </c>
     </row>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>7211243743205361964</t>
+          <t>6101353054216547389</t>
         </is>
       </c>
     </row>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>-1397029152657909876</t>
+          <t>-1728161483433841628</t>
         </is>
       </c>
     </row>
@@ -7499,7 +7499,7 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>-2957664614295267829</t>
+          <t>7800114793456783754</t>
         </is>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>-1019300093287602957</t>
+          <t>2822999976005657376</t>
         </is>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>5083804542754861460</t>
+          <t>7984650632942063071</t>
         </is>
       </c>
     </row>
@@ -7673,7 +7673,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>-684667185360629911</t>
+          <t>-5340742443449096831</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>2181380623218178445</t>
+          <t>-5593536686870893561</t>
         </is>
       </c>
     </row>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>8595903504432045558</t>
+          <t>7081424173988031957</t>
         </is>
       </c>
     </row>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>-1819096483199804492</t>
+          <t>-5760122561434536915</t>
         </is>
       </c>
     </row>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>-2522337984013915347</t>
+          <t>-2480073769315132220</t>
         </is>
       </c>
     </row>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>-3447057015283101846</t>
+          <t>-1855349223466020015</t>
         </is>
       </c>
     </row>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>1715740541100954805</t>
+          <t>3320656996543785179</t>
         </is>
       </c>
     </row>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>-8336191736962316114</t>
+          <t>3897800154192342689</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>1530903909874727812</t>
+          <t>353991244668419229</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>-6617530120066595529</t>
+          <t>-5899110517733048259</t>
         </is>
       </c>
     </row>
@@ -8247,7 +8247,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>-3630915378332725157</t>
+          <t>-8198737688466134131</t>
         </is>
       </c>
     </row>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>6766916804570629763</t>
+          <t>6612813257336915871</t>
         </is>
       </c>
     </row>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>-6102625487373628845</t>
+          <t>5915562354588149636</t>
         </is>
       </c>
     </row>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>-6427175365258669468</t>
+          <t>1370250394654787236</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>8868946038062910910</t>
+          <t>4359501372916182163</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>7595204490086872621</t>
+          <t>-9004078259337114266</t>
         </is>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>-2207655033940450072</t>
+          <t>-1581356058148466009</t>
         </is>
       </c>
     </row>
@@ -8653,7 +8653,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>-4322783782782921251</t>
+          <t>-187559124536684712</t>
         </is>
       </c>
     </row>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>-231162873458323514</t>
+          <t>-7096599675213249758</t>
         </is>
       </c>
     </row>
@@ -8769,7 +8769,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>7050037241090277956</t>
+          <t>5769468660976733518</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>-7873238011731733162</t>
+          <t>3960571449355336873</t>
         </is>
       </c>
     </row>
@@ -8881,7 +8881,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>-5941049182536849109</t>
+          <t>-8777393734123867828</t>
         </is>
       </c>
     </row>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>-8620407933545991259</t>
+          <t>9008536352740260377</t>
         </is>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>-559472240420349259</t>
+          <t>-8241586007594652290</t>
         </is>
       </c>
     </row>
@@ -9055,7 +9055,7 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>-4981140518067300793</t>
+          <t>-8222123172699938240</t>
         </is>
       </c>
     </row>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>643542772026338771</t>
+          <t>-92094463202918188</t>
         </is>
       </c>
     </row>
@@ -9167,7 +9167,7 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>3268863545090775617</t>
+          <t>5399163550283359428</t>
         </is>
       </c>
     </row>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>2672343686471530480</t>
+          <t>3278444896356932343</t>
         </is>
       </c>
     </row>
@@ -9279,7 +9279,7 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>-3643599378168043464</t>
+          <t>4879536268522119789</t>
         </is>
       </c>
     </row>
@@ -9335,7 +9335,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>6434209926653554900</t>
+          <t>-3915506919362854791</t>
         </is>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>-1270118825763535676</t>
+          <t>-3606897734813795456</t>
         </is>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>5429892603301549684</t>
+          <t>8080441122919786149</t>
         </is>
       </c>
     </row>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>-8894611048198543196</t>
+          <t>-3682793629583041216</t>
         </is>
       </c>
     </row>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>-2160264276138159527</t>
+          <t>362708061386542852</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>-8474327674694741285</t>
+          <t>7137277816952640698</t>
         </is>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>246140732267578233</t>
+          <t>-7943750480362147549</t>
         </is>
       </c>
     </row>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>-1129151466573563612</t>
+          <t>186926011229381055</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>9205179774127900571</t>
+          <t>4989294705057204297</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>-2364160728764779491</t>
+          <t>-5445347898362226560</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>8108395386256394258</t>
+          <t>6586420778007030458</t>
         </is>
       </c>
     </row>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>-954166402165324989</t>
+          <t>8063619828418241439</t>
         </is>
       </c>
     </row>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>543821272980740781</t>
+          <t>-734695181698216634</t>
         </is>
       </c>
     </row>
@@ -10081,7 +10081,7 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>8546088309797410840</t>
+          <t>-5197983080205380048</t>
         </is>
       </c>
     </row>
@@ -10139,7 +10139,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>444406988666437715</t>
+          <t>8771397794407928550</t>
         </is>
       </c>
     </row>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>6674371758819296065</t>
+          <t>2758463715666977132</t>
         </is>
       </c>
     </row>
@@ -10253,7 +10253,7 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>-5504371936227284663</t>
+          <t>-7629228907632249850</t>
         </is>
       </c>
     </row>
@@ -10309,7 +10309,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>6352385770273794128</t>
+          <t>-6013129583260605860</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>-9032907689358954166</t>
+          <t>1706544054168619428</t>
         </is>
       </c>
     </row>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>-6541113570474471252</t>
+          <t>5908544284071976582</t>
         </is>
       </c>
     </row>
@@ -10479,7 +10479,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>1401012005982569654</t>
+          <t>-8252943318095842865</t>
         </is>
       </c>
     </row>
@@ -10537,7 +10537,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>-1292458585129911830</t>
+          <t>8162587067926169803</t>
         </is>
       </c>
     </row>
@@ -10595,7 +10595,7 @@
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>8697378646641891277</t>
+          <t>-6923344614904924950</t>
         </is>
       </c>
     </row>
@@ -10653,7 +10653,7 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>6179180593092849479</t>
+          <t>-5710788152847396953</t>
         </is>
       </c>
     </row>
@@ -10711,7 +10711,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>6365682726562351476</t>
+          <t>5441018582480530680</t>
         </is>
       </c>
     </row>
@@ -10769,7 +10769,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>8164388562393133545</t>
+          <t>151897295708100348</t>
         </is>
       </c>
     </row>
@@ -10827,7 +10827,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>-721850228734678966</t>
+          <t>3753925023441383226</t>
         </is>
       </c>
     </row>
@@ -10885,7 +10885,7 @@
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>-8049177185306195896</t>
+          <t>-3080955197613403790</t>
         </is>
       </c>
     </row>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>-6309357319046325101</t>
+          <t>2497427562318075770</t>
         </is>
       </c>
     </row>
@@ -10997,7 +10997,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>-518677825884927479</t>
+          <t>4980733130656200362</t>
         </is>
       </c>
     </row>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>-6928029703104404322</t>
+          <t>5556780101110100077</t>
         </is>
       </c>
     </row>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>4579203732849881173</t>
+          <t>-5631845252436758871</t>
         </is>
       </c>
     </row>
@@ -11171,7 +11171,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>5728739737985536577</t>
+          <t>1389582937354381361</t>
         </is>
       </c>
     </row>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>8216443390237770815</t>
+          <t>-3246581684170894781</t>
         </is>
       </c>
     </row>
@@ -11283,7 +11283,7 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>1278822940952494633</t>
+          <t>-1186033979660594061</t>
         </is>
       </c>
     </row>
@@ -11339,7 +11339,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>4005647799575941891</t>
+          <t>3425714549761616657</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaned the agent a response ui
</commit_message>
<xml_diff>
--- a/data/Resources Version 3.xlsx
+++ b/data/Resources Version 3.xlsx
@@ -547,7 +547,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>3662640957984824165</t>
+          <t>2304868239367260535</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>-2205727469830209581</t>
+          <t>-583762912206321705</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>3947032688143015583</t>
+          <t>8785402743548180080</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>-4070058339261262404</t>
+          <t>3400124436684708168</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>3974254717169165242</t>
+          <t>-9050484981951592694</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-4561709708017358982</t>
+          <t>-4943325104946250972</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>1551291109968057236</t>
+          <t>1424988354000457463</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>-4518089163609736458</t>
+          <t>-5957504402761910113</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>-3183684730125675937</t>
+          <t>-3435909194036863436</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-9168276457019987318</t>
+          <t>4354667135340456543</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>-4617949069363649069</t>
+          <t>-1322137600156062817</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>3493635241480552645</t>
+          <t>-4620310552291491404</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>4120352725638207378</t>
+          <t>8104143319666563102</t>
         </is>
       </c>
     </row>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>1520873511535781825</t>
+          <t>7657496261720818359</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>6574711592521513742</t>
+          <t>-4907139835942571568</t>
         </is>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>-8338804174920443849</t>
+          <t>-4042432392241163074</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>312702367421235649</t>
+          <t>-4668876104820315357</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>-5970054463927394358</t>
+          <t>-3700254585904948443</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>-4263260082488223738</t>
+          <t>5842244297029825491</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>-5612201309808146888</t>
+          <t>4644045229442236511</t>
         </is>
       </c>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>5145432123831290462</t>
+          <t>-4574849836526349793</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>1015697036543477830</t>
+          <t>-1710727394617431640</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>-208326485726242567</t>
+          <t>-8089276158946786017</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>7646751089657057711</t>
+          <t>-191897296091881875</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>-5415919449685052607</t>
+          <t>1377657537058853721</t>
         </is>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>7868390111142095063</t>
+          <t>-6169861955316812718</t>
         </is>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>-7488405086253764194</t>
+          <t>3790630249376912635</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>-1861682879708476291</t>
+          <t>6692488160665585693</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>-8847728220741545953</t>
+          <t>4317145232798592146</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>4457302807822112719</t>
+          <t>-1302224202447775013</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>-625322754259993442</t>
+          <t>2580386303136802540</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>-3213279485514674737</t>
+          <t>-3998316194452072514</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>8404831805550815693</t>
+          <t>2183031812100989262</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>-8933857045255588965</t>
+          <t>-3278855361572786632</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>5254168911598103324</t>
+          <t>1681143363934357293</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>-772281424943873119</t>
+          <t>2797402779549644328</t>
         </is>
       </c>
     </row>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>5497686737915771151</t>
+          <t>4095904084766668235</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>-8007489703386405862</t>
+          <t>-276851183466949714</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>-1224088264320340539</t>
+          <t>1163287500519352989</t>
         </is>
       </c>
     </row>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>65550805372217523</t>
+          <t>4981040301797692386</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>3959022303982822678</t>
+          <t>8454626419971359385</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2893424119587123128</t>
+          <t>-8440630127675969930</t>
         </is>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>6729436500093376029</t>
+          <t>4185285982014713493</t>
         </is>
       </c>
     </row>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>-9092111020908679666</t>
+          <t>6118134113576469429</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>-5776440433675510743</t>
+          <t>6628599794655278238</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>3289512220574743916</t>
+          <t>-8231369234022507766</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>-3912504612805688163</t>
+          <t>-6054229867113545513</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>211745950761418373</t>
+          <t>1535812957976389961</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>-813659942172640462</t>
+          <t>-4257047721384202478</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>-280881007667315352</t>
+          <t>-7028354771250386908</t>
         </is>
       </c>
     </row>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>-637642966314824375</t>
+          <t>7138504405051230327</t>
         </is>
       </c>
     </row>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>4018800685974547100</t>
+          <t>-3742014445397112650</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>6425201151129509066</t>
+          <t>7569486917987237219</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>664692401615066690</t>
+          <t>2868508394872918775</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>1575136103729739998</t>
+          <t>-2255850828834310092</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>-2557687514756119600</t>
+          <t>-1291348957807049971</t>
         </is>
       </c>
     </row>
@@ -3755,7 +3755,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>-4299873427710969298</t>
+          <t>-2785877888075745551</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>-940197697172272793</t>
+          <t>1018876795810679842</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>-6794072827604301818</t>
+          <t>-7899525107786530249</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>-8673794620469508205</t>
+          <t>5942658507352084174</t>
         </is>
       </c>
     </row>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>-781131645495908453</t>
+          <t>-3070291095952211113</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>-1330214522552559642</t>
+          <t>-2253876670091193342</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>5774951135724176630</t>
+          <t>-4747966684282186950</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>-2492042789545590560</t>
+          <t>-19910544688683300</t>
         </is>
       </c>
     </row>
@@ -4205,7 +4205,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>5165846990965736332</t>
+          <t>5321017328663793403</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4261,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>3130469186114237930</t>
+          <t>-5293885784838247343</t>
         </is>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>-774411147450069977</t>
+          <t>-6001519506611179400</t>
         </is>
       </c>
     </row>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>-2650407188651912047</t>
+          <t>5478372927738525128</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>-908987616845626214</t>
+          <t>6940864072629015760</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>-4060061898629540777</t>
+          <t>8479967176440715432</t>
         </is>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>-4532436151914642469</t>
+          <t>-8622078424782469548</t>
         </is>
       </c>
     </row>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>1459852186908969580</t>
+          <t>-2934783846717936329</t>
         </is>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>6282601747389355345</t>
+          <t>-2236752232088142139</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>3519689203908794831</t>
+          <t>8321305845499732755</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>1638720622492765062</t>
+          <t>-5829710602110292443</t>
         </is>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>-8033667434504302137</t>
+          <t>-2265489032386565619</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>6751182094598153038</t>
+          <t>7839770625195447432</t>
         </is>
       </c>
     </row>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>-5254112671037145471</t>
+          <t>-5864609994055273740</t>
         </is>
       </c>
     </row>
@@ -5001,7 +5001,7 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>1076389866509198222</t>
+          <t>-5334434868151123154</t>
         </is>
       </c>
     </row>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>-2962127134674495331</t>
+          <t>1855026219238267671</t>
         </is>
       </c>
     </row>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>-4919118608278039778</t>
+          <t>-2990424921668602334</t>
         </is>
       </c>
     </row>
@@ -5171,7 +5171,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>-7231451410249793031</t>
+          <t>-8252934711208658664</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>1605600418937571350</t>
+          <t>-6685604864765827358</t>
         </is>
       </c>
     </row>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>917846148114197462</t>
+          <t>3300140167683451205</t>
         </is>
       </c>
     </row>
@@ -5343,7 +5343,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>-6364450786823172080</t>
+          <t>-6166394640839655179</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>2924035588330404652</t>
+          <t>1106017260565123439</t>
         </is>
       </c>
     </row>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>-5769097701753140988</t>
+          <t>-3271996208110276461</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>-8827049855292318136</t>
+          <t>4900525386176276760</t>
         </is>
       </c>
     </row>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>4173045203913581098</t>
+          <t>-1074436845531276588</t>
         </is>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>-5278319329484131655</t>
+          <t>8326582088608019008</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>-1735731827933621612</t>
+          <t>2216915330005314130</t>
         </is>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>1952093456905376577</t>
+          <t>474765205137979292</t>
         </is>
       </c>
     </row>
@@ -5799,7 +5799,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>2173678999482831795</t>
+          <t>5616698105353656014</t>
         </is>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>5900994253310099602</t>
+          <t>5497862162795429203</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>5468280461743058903</t>
+          <t>-7409765893085170494</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>5992219105724045985</t>
+          <t>2322459821782056968</t>
         </is>
       </c>
     </row>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>-855068379621288064</t>
+          <t>-7386670263333217762</t>
         </is>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>-7514884896793776053</t>
+          <t>3587310744116981750</t>
         </is>
       </c>
     </row>
@@ -6135,7 +6135,7 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>-4007255360055736767</t>
+          <t>-8904602195075027020</t>
         </is>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>9051414917383599879</t>
+          <t>-9189718269616821820</t>
         </is>
       </c>
     </row>
@@ -6247,7 +6247,7 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>-1180506624026339843</t>
+          <t>6772467600022404810</t>
         </is>
       </c>
     </row>
@@ -6303,7 +6303,7 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>-857840874557669554</t>
+          <t>-4670903865598048557</t>
         </is>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>-3207098703688345024</t>
+          <t>630777240695058317</t>
         </is>
       </c>
     </row>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>-6880334182832083659</t>
+          <t>6934030370542940517</t>
         </is>
       </c>
     </row>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>-43504159787510576</t>
+          <t>-4682087002096336199</t>
         </is>
       </c>
     </row>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>101705950246348686</t>
+          <t>-5723817821506187717</t>
         </is>
       </c>
     </row>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>-7616530941552643312</t>
+          <t>5660628859891988374</t>
         </is>
       </c>
     </row>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="L109" t="inlineStr">
         <is>
-          <t>-7243990865538090742</t>
+          <t>-7468771989873465520</t>
         </is>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>-6331353430656479257</t>
+          <t>756838708080843586</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>8261618368864195616</t>
+          <t>9116532671958360029</t>
         </is>
       </c>
     </row>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>-4462920339258683482</t>
+          <t>4383452453679466998</t>
         </is>
       </c>
     </row>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="L113" t="inlineStr">
         <is>
-          <t>1002060103863177932</t>
+          <t>-3634604571585369254</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>-8158071597057416025</t>
+          <t>-7513217818182624704</t>
         </is>
       </c>
     </row>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>-8157904845361839123</t>
+          <t>3997276097851215677</t>
         </is>
       </c>
     </row>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>-6026434707399987736</t>
+          <t>8736461469028132443</t>
         </is>
       </c>
     </row>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>5596896287552915416</t>
+          <t>-411171869757592416</t>
         </is>
       </c>
     </row>
@@ -7161,7 +7161,7 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>7014636261738343865</t>
+          <t>6619254962465997494</t>
         </is>
       </c>
     </row>
@@ -7217,7 +7217,7 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>-1621598255050098166</t>
+          <t>-8683652262124824405</t>
         </is>
       </c>
     </row>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>1765071489886768529</t>
+          <t>3810370592045271121</t>
         </is>
       </c>
     </row>
@@ -7331,7 +7331,7 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>-1644948235369330338</t>
+          <t>4197014717401158349</t>
         </is>
       </c>
     </row>
@@ -7387,7 +7387,7 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>6101353054216547389</t>
+          <t>-2100923059394626847</t>
         </is>
       </c>
     </row>
@@ -7443,7 +7443,7 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>-1728161483433841628</t>
+          <t>2767387746887664777</t>
         </is>
       </c>
     </row>
@@ -7499,7 +7499,7 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>7800114793456783754</t>
+          <t>-2517668809775098545</t>
         </is>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>2822999976005657376</t>
+          <t>-5517995399047614983</t>
         </is>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>7984650632942063071</t>
+          <t>-1172261524025422549</t>
         </is>
       </c>
     </row>
@@ -7673,7 +7673,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>-5340742443449096831</t>
+          <t>3823555205836393339</t>
         </is>
       </c>
     </row>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>-5593536686870893561</t>
+          <t>-3025837833948824392</t>
         </is>
       </c>
     </row>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>7081424173988031957</t>
+          <t>8757545355424537928</t>
         </is>
       </c>
     </row>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>-5760122561434536915</t>
+          <t>3800805685194110061</t>
         </is>
       </c>
     </row>
@@ -7901,7 +7901,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>-2480073769315132220</t>
+          <t>5879217366379764520</t>
         </is>
       </c>
     </row>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>-1855349223466020015</t>
+          <t>-5220888266976836830</t>
         </is>
       </c>
     </row>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>3320656996543785179</t>
+          <t>6732999641629727996</t>
         </is>
       </c>
     </row>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>3897800154192342689</t>
+          <t>5671680652438995972</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>353991244668419229</t>
+          <t>6341911288258650433</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>-5899110517733048259</t>
+          <t>-9103379384387054510</t>
         </is>
       </c>
     </row>
@@ -8247,7 +8247,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>-8198737688466134131</t>
+          <t>7166361720806085764</t>
         </is>
       </c>
     </row>
@@ -8305,7 +8305,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>6612813257336915871</t>
+          <t>-4796240225206165461</t>
         </is>
       </c>
     </row>
@@ -8363,7 +8363,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>5915562354588149636</t>
+          <t>-6144910809346714597</t>
         </is>
       </c>
     </row>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>1370250394654787236</t>
+          <t>683544569499197146</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>4359501372916182163</t>
+          <t>4762640626829788335</t>
         </is>
       </c>
     </row>
@@ -8537,7 +8537,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>-9004078259337114266</t>
+          <t>-1337093275511199398</t>
         </is>
       </c>
     </row>
@@ -8595,7 +8595,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>-1581356058148466009</t>
+          <t>-2249309194168929568</t>
         </is>
       </c>
     </row>
@@ -8653,7 +8653,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>-187559124536684712</t>
+          <t>-2093888654028549874</t>
         </is>
       </c>
     </row>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>-7096599675213249758</t>
+          <t>-2845360229156491663</t>
         </is>
       </c>
     </row>
@@ -8769,7 +8769,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>5769468660976733518</t>
+          <t>2251348352273863068</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>3960571449355336873</t>
+          <t>2100078293069603737</t>
         </is>
       </c>
     </row>
@@ -8881,7 +8881,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>-8777393734123867828</t>
+          <t>443643041691075247</t>
         </is>
       </c>
     </row>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>9008536352740260377</t>
+          <t>6021440198355577087</t>
         </is>
       </c>
     </row>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>-8241586007594652290</t>
+          <t>-4588723334104686355</t>
         </is>
       </c>
     </row>
@@ -9055,7 +9055,7 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>-8222123172699938240</t>
+          <t>-3136693748195056644</t>
         </is>
       </c>
     </row>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>-92094463202918188</t>
+          <t>-5021477324580289772</t>
         </is>
       </c>
     </row>
@@ -9167,7 +9167,7 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>5399163550283359428</t>
+          <t>-7472008825738386908</t>
         </is>
       </c>
     </row>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>3278444896356932343</t>
+          <t>4340758081371250521</t>
         </is>
       </c>
     </row>
@@ -9279,7 +9279,7 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>4879536268522119789</t>
+          <t>-917419165160168540</t>
         </is>
       </c>
     </row>
@@ -9335,7 +9335,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>-3915506919362854791</t>
+          <t>6890702430602127789</t>
         </is>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>-3606897734813795456</t>
+          <t>1870363055048317126</t>
         </is>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>8080441122919786149</t>
+          <t>4123511959377508674</t>
         </is>
       </c>
     </row>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>-3682793629583041216</t>
+          <t>-965986892309267371</t>
         </is>
       </c>
     </row>
@@ -9567,7 +9567,7 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>362708061386542852</t>
+          <t>-500551395573698225</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>7137277816952640698</t>
+          <t>8613135478478487629</t>
         </is>
       </c>
     </row>
@@ -9681,7 +9681,7 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>-7943750480362147549</t>
+          <t>1392547041859570903</t>
         </is>
       </c>
     </row>
@@ -9739,7 +9739,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>186926011229381055</t>
+          <t>5892542477041407556</t>
         </is>
       </c>
     </row>
@@ -9795,7 +9795,7 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>4989294705057204297</t>
+          <t>6571141281251410123</t>
         </is>
       </c>
     </row>
@@ -9851,7 +9851,7 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>-5445347898362226560</t>
+          <t>-3216547748641616728</t>
         </is>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>6586420778007030458</t>
+          <t>4190276734838983307</t>
         </is>
       </c>
     </row>
@@ -9967,7 +9967,7 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>8063619828418241439</t>
+          <t>-6270638751622077169</t>
         </is>
       </c>
     </row>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>-734695181698216634</t>
+          <t>-4221004449911767743</t>
         </is>
       </c>
     </row>
@@ -10081,7 +10081,7 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>-5197983080205380048</t>
+          <t>-219137094125268342</t>
         </is>
       </c>
     </row>
@@ -10139,7 +10139,7 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>8771397794407928550</t>
+          <t>-1969798909350897427</t>
         </is>
       </c>
     </row>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>2758463715666977132</t>
+          <t>258564560753389072</t>
         </is>
       </c>
     </row>
@@ -10253,7 +10253,7 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>-7629228907632249850</t>
+          <t>-588547858700785154</t>
         </is>
       </c>
     </row>
@@ -10309,7 +10309,7 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>-6013129583260605860</t>
+          <t>-972701403886747948</t>
         </is>
       </c>
     </row>
@@ -10365,7 +10365,7 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>1706544054168619428</t>
+          <t>-2601218650283546222</t>
         </is>
       </c>
     </row>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>5908544284071976582</t>
+          <t>-4841276781346413664</t>
         </is>
       </c>
     </row>
@@ -10479,7 +10479,7 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>-8252943318095842865</t>
+          <t>1179990251309205443</t>
         </is>
       </c>
     </row>
@@ -10537,7 +10537,7 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>8162587067926169803</t>
+          <t>-5417459133772220954</t>
         </is>
       </c>
     </row>
@@ -10595,7 +10595,7 @@
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>-6923344614904924950</t>
+          <t>-1557897592802345440</t>
         </is>
       </c>
     </row>
@@ -10653,7 +10653,7 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>-5710788152847396953</t>
+          <t>-4149379874577191353</t>
         </is>
       </c>
     </row>
@@ -10711,7 +10711,7 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>5441018582480530680</t>
+          <t>8021212652910037478</t>
         </is>
       </c>
     </row>
@@ -10769,7 +10769,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>151897295708100348</t>
+          <t>5428655001110708489</t>
         </is>
       </c>
     </row>
@@ -10827,7 +10827,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>3753925023441383226</t>
+          <t>-5321196204213227204</t>
         </is>
       </c>
     </row>
@@ -10885,7 +10885,7 @@
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>-3080955197613403790</t>
+          <t>-8186922673451443675</t>
         </is>
       </c>
     </row>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>2497427562318075770</t>
+          <t>6092103733379781598</t>
         </is>
       </c>
     </row>
@@ -10997,7 +10997,7 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>4980733130656200362</t>
+          <t>-3006421748206221594</t>
         </is>
       </c>
     </row>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>5556780101110100077</t>
+          <t>-5878807307924458713</t>
         </is>
       </c>
     </row>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>-5631845252436758871</t>
+          <t>-6719619109426543157</t>
         </is>
       </c>
     </row>
@@ -11171,7 +11171,7 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>1389582937354381361</t>
+          <t>1325636250299665191</t>
         </is>
       </c>
     </row>
@@ -11227,7 +11227,7 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>-3246581684170894781</t>
+          <t>7480592257608434379</t>
         </is>
       </c>
     </row>
@@ -11283,7 +11283,7 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>-1186033979660594061</t>
+          <t>7092530563699290161</t>
         </is>
       </c>
     </row>
@@ -11339,7 +11339,7 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>3425714549761616657</t>
+          <t>-6937588045200454942</t>
         </is>
       </c>
     </row>

</xml_diff>